<commit_message>
Updated pages "AES cipher internals in Excel", "DES cipher internals in Excel".
</commit_message>
<xml_diff>
--- a/aes-cipher-internals-in-excel/aes-cipher-internals.xlsx
+++ b/aes-cipher-internals-in-excel/aes-cipher-internals.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AES-128" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="AES-128 Decrypt" sheetId="5" r:id="rId4"/>
     <sheet name="Tables" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -941,9 +941,6 @@
     <t>Round 14</t>
   </si>
   <si>
-    <t>Copyright © 2013 Nayuki Minase</t>
-  </si>
-  <si>
     <t>S-box inverse</t>
   </si>
   <si>
@@ -965,9 +962,6 @@
     <t>AES-128 Decryption Internals</t>
   </si>
   <si>
-    <t>Copyright © 2016 Nayuki Minase</t>
-  </si>
-  <si>
     <t>Ciphertext (input)</t>
   </si>
   <si>
@@ -975,12 +969,18 @@
   </si>
   <si>
     <t>https://www.nayuki.io/page/aes-cipher-internals-in-excel</t>
+  </si>
+  <si>
+    <t>Copyright © 2013 Project Nayuki</t>
+  </si>
+  <si>
+    <t>Copyright © 2016 Project Nayuki</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1239,25 +1239,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1275,10 +1263,22 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1384,6 +1384,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1419,6 +1436,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1594,7 +1628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -1610,98 +1644,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
     </row>
     <row r="2" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40" t="s">
-        <v>318</v>
-      </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
+      <c r="A2" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
     </row>
     <row r="3" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39" t="s">
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="O4" s="47" t="s">
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="O4" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="47"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
     </row>
     <row r="5" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
@@ -1744,22 +1778,22 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="O5" s="35" t="s">
+      <c r="O5" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35" t="str">
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34" t="str">
         <f>CONCATENATE(B5,B6,B7,B8,C5,C6,C7,C8,D5,D6,D7,D8,E5,E6,E7,E8)</f>
         <v>3243F6A8885A308D313198A2E0370734</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
     </row>
     <row r="6" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
@@ -1802,22 +1836,22 @@
         <f t="shared" si="0"/>
         <v>6A</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35" t="str">
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34" t="str">
         <f>CONCATENATE(F5,F6,F7,F8,G5,G6,G7,G8,H5,H6,H7,H8,I5,I6,I7,I8)</f>
         <v>2B7E151628AED2A6ABF7158809CF4F3C</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
     </row>
     <row r="7" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
@@ -1860,22 +1894,22 @@
         <f t="shared" si="0"/>
         <v>0B</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="35" t="str">
+      <c r="P7" s="35"/>
+      <c r="Q7" s="34" t="str">
         <f>CONCATENATE(J5,J6,J7,J8,K5,K6,K7,K8,L5,L6,L7,L8,M5,M6,M7,M8)</f>
         <v>3925841D02DC09FBDC118597196A0B32</v>
       </c>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
     </row>
     <row r="8" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
@@ -1928,42 +1962,42 @@
     </row>
     <row r="10" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="36" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="36" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37" t="s">
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="41" t="s">
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
     </row>
     <row r="11" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -5627,50 +5661,53 @@
     </row>
     <row r="55" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="43" t="s">
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="42" t="s">
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="44"/>
-      <c r="N55" s="43" t="s">
+      <c r="K55" s="39"/>
+      <c r="L55" s="39"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="O55" s="43"/>
-      <c r="P55" s="43"/>
-      <c r="Q55" s="43"/>
-      <c r="R55" s="42" t="s">
+      <c r="O55" s="39"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="39"/>
+      <c r="R55" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="S55" s="43"/>
-      <c r="T55" s="43"/>
-      <c r="U55" s="44"/>
-      <c r="V55" s="45" t="s">
+      <c r="S55" s="39"/>
+      <c r="T55" s="39"/>
+      <c r="U55" s="40"/>
+      <c r="V55" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="W55" s="45"/>
-      <c r="X55" s="45"/>
-      <c r="Y55" s="45"/>
+      <c r="W55" s="41"/>
+      <c r="X55" s="41"/>
+      <c r="Y55" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="Q7:Y7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O4:Y4"/>
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="Q5:Y5"/>
+    <mergeCell ref="Q6:Y6"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:Y2"/>
     <mergeCell ref="V10:Y10"/>
     <mergeCell ref="B55:E55"/>
     <mergeCell ref="F55:I55"/>
@@ -5683,14 +5720,11 @@
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="R10:U10"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="Q5:Y5"/>
-    <mergeCell ref="Q6:Y6"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:Y2"/>
+    <mergeCell ref="Q7:Y7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5698,7 +5732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5714,100 +5748,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
     </row>
     <row r="2" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40" t="s">
-        <v>318</v>
-      </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
+      <c r="A2" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
     </row>
     <row r="3" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="38"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="44"/>
       <c r="L4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="Q4" s="47" t="s">
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="Q4" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="47"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="47"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
     </row>
     <row r="5" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
@@ -5856,22 +5890,22 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="Q5" s="35" t="s">
+      <c r="Q5" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35" t="str">
+      <c r="R5" s="34"/>
+      <c r="S5" s="34" t="str">
         <f>CONCATENATE(B5,B6,B7,B8,C5,C6,C7,C8,D5,D6,D7,D8,E5,E6,E7,E8)</f>
         <v>6BC1BEE22E409F96E93D7E117393172A</v>
       </c>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
-      <c r="AA5" s="35"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
     </row>
     <row r="6" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
@@ -5920,26 +5954,26 @@
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="Q6" s="35" t="s">
+      <c r="Q6" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35" t="str">
+      <c r="R6" s="34"/>
+      <c r="S6" s="34" t="str">
         <f>CONCATENATE(F5,F6,F7,F8,G5,G6,G7,G8,H5,H6,H7,H8,I5,I6,I7,I8,J5,J6,J7,J8,K5,K6,K7,K8)</f>
         <v>8E73B0F7DA0E6452C810F32B809079E562F8EAD2522C6B7B</v>
       </c>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="35"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="34"/>
+      <c r="AC6" s="34"/>
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="34"/>
     </row>
     <row r="7" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
@@ -5988,22 +6022,22 @@
         <f t="shared" si="0"/>
         <v>A5</v>
       </c>
-      <c r="Q7" s="46" t="s">
+      <c r="Q7" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="R7" s="46"/>
-      <c r="S7" s="35" t="str">
+      <c r="R7" s="35"/>
+      <c r="S7" s="34" t="str">
         <f>CONCATENATE(L5,L6,L7,L8,M5,M6,M7,M8,N5,N6,N7,N8,O5,O6,O7,O8)</f>
         <v>BD334F1D6E45F25FF712A214571FA5CC</v>
       </c>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="35"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34"/>
     </row>
     <row r="8" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
@@ -6066,42 +6100,42 @@
     </row>
     <row r="10" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="36" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="36" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37" t="s">
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="41" t="s">
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
     </row>
     <row r="11" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -10458,45 +10492,54 @@
     </row>
     <row r="63" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="43" t="s">
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="42" t="s">
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="K63" s="43"/>
-      <c r="L63" s="43"/>
-      <c r="M63" s="44"/>
-      <c r="N63" s="43" t="s">
+      <c r="K63" s="39"/>
+      <c r="L63" s="39"/>
+      <c r="M63" s="40"/>
+      <c r="N63" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="O63" s="43"/>
-      <c r="P63" s="43"/>
-      <c r="Q63" s="43"/>
-      <c r="R63" s="42" t="s">
+      <c r="O63" s="39"/>
+      <c r="P63" s="39"/>
+      <c r="Q63" s="39"/>
+      <c r="R63" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="S63" s="43"/>
-      <c r="T63" s="43"/>
-      <c r="U63" s="44"/>
-      <c r="V63" s="45" t="s">
+      <c r="S63" s="39"/>
+      <c r="T63" s="39"/>
+      <c r="U63" s="40"/>
+      <c r="V63" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="W63" s="45"/>
-      <c r="X63" s="45"/>
-      <c r="Y63" s="45"/>
+      <c r="W63" s="41"/>
+      <c r="X63" s="41"/>
+      <c r="Y63" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="Q4:AA4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:Y2"/>
     <mergeCell ref="S6:AE6"/>
     <mergeCell ref="B63:E63"/>
     <mergeCell ref="F63:I63"/>
@@ -10513,15 +10556,6 @@
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="R10:U10"/>
     <mergeCell ref="V10:Y10"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="Q4:AA4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:AA5"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10529,7 +10563,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -10545,102 +10579,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
     </row>
     <row r="2" spans="1:37" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40" t="s">
-        <v>318</v>
-      </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
+      <c r="A2" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
     </row>
     <row r="3" spans="1:37" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="38"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="44"/>
       <c r="N4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="S4" s="47" t="s">
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="S4" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="47"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="47"/>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
     </row>
     <row r="5" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
@@ -10695,22 +10729,22 @@
         <f t="shared" si="0"/>
         <v>3D</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35" t="str">
+      <c r="T5" s="34"/>
+      <c r="U5" s="34" t="str">
         <f>CONCATENATE(B5,B6,B7,B8,C5,C6,C7,C8,D5,D6,D7,D8,E5,E6,E7,E8)</f>
         <v>6BC1BEE22E409F96E93D7E117393172A</v>
       </c>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="35"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
     </row>
     <row r="6" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
@@ -10765,30 +10799,30 @@
         <f t="shared" si="2"/>
         <v>B1</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35" t="str">
+      <c r="T6" s="34"/>
+      <c r="U6" s="34" t="str">
         <f>CONCATENATE(F5,F6,F7,F8,G5,G6,G7,G8,H5,H6,H7,H8,I5,I6,I7,I8,J5,J6,J7,J8,K5,K6,K7,K8,L5,L6,L7,L8,M5,M6,M7,M8)</f>
         <v>603DEB1015CA71BE2B73AEF0857D77811F352C073B6108D72D9810A30914DFF4</v>
       </c>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="35"/>
-      <c r="AF6" s="35"/>
-      <c r="AG6" s="35"/>
-      <c r="AH6" s="35"/>
-      <c r="AI6" s="35"/>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="35"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="34"/>
+      <c r="AC6" s="34"/>
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="34"/>
+      <c r="AF6" s="34"/>
+      <c r="AG6" s="34"/>
+      <c r="AH6" s="34"/>
+      <c r="AI6" s="34"/>
+      <c r="AJ6" s="34"/>
+      <c r="AK6" s="34"/>
     </row>
     <row r="7" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
@@ -10843,22 +10877,22 @@
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
-      <c r="S7" s="46" t="s">
+      <c r="S7" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="T7" s="46"/>
-      <c r="U7" s="35" t="str">
+      <c r="T7" s="35"/>
+      <c r="U7" s="34" t="str">
         <f>CONCATENATE(N5,N6,N7,N8,O5,O6,O7,O8,P5,P6,P7,P8,Q5,Q6,Q7,Q8)</f>
         <v>F3EED1BDB5D2A03C064B5A7E3DB181F8</v>
       </c>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="35"/>
-      <c r="AC7" s="35"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="34"/>
     </row>
     <row r="8" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
@@ -10931,42 +10965,42 @@
     </row>
     <row r="10" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="36" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="36" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37" t="s">
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="41" t="s">
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
     </row>
     <row r="11" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -16018,54 +16052,45 @@
     </row>
     <row r="71" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
-      <c r="B71" s="42" t="s">
+      <c r="B71" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C71" s="43"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="43" t="s">
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G71" s="43"/>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
-      <c r="J71" s="42" t="s">
+      <c r="G71" s="39"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="39"/>
+      <c r="J71" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="K71" s="43"/>
-      <c r="L71" s="43"/>
-      <c r="M71" s="44"/>
-      <c r="N71" s="43" t="s">
+      <c r="K71" s="39"/>
+      <c r="L71" s="39"/>
+      <c r="M71" s="40"/>
+      <c r="N71" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="O71" s="43"/>
-      <c r="P71" s="43"/>
-      <c r="Q71" s="43"/>
-      <c r="R71" s="42" t="s">
+      <c r="O71" s="39"/>
+      <c r="P71" s="39"/>
+      <c r="Q71" s="39"/>
+      <c r="R71" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="S71" s="43"/>
-      <c r="T71" s="43"/>
-      <c r="U71" s="44"/>
-      <c r="V71" s="45" t="s">
+      <c r="S71" s="39"/>
+      <c r="T71" s="39"/>
+      <c r="U71" s="40"/>
+      <c r="V71" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="W71" s="45"/>
-      <c r="X71" s="45"/>
-      <c r="Y71" s="45"/>
+      <c r="W71" s="41"/>
+      <c r="X71" s="41"/>
+      <c r="Y71" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:Y2"/>
-    <mergeCell ref="U5:AC5"/>
-    <mergeCell ref="S4:AC4"/>
-    <mergeCell ref="U7:AC7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U6:AK6"/>
     <mergeCell ref="A1:Y1"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="N4:Q4"/>
@@ -16082,6 +16107,15 @@
     <mergeCell ref="J71:M71"/>
     <mergeCell ref="N71:Q71"/>
     <mergeCell ref="R71:U71"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:Y2"/>
+    <mergeCell ref="U5:AC5"/>
+    <mergeCell ref="S4:AC4"/>
+    <mergeCell ref="U7:AC7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U6:AK6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16089,7 +16123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -16105,98 +16139,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
+      <c r="A1" s="45" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
     </row>
     <row r="2" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>315</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40" t="s">
+      <c r="A2" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
     </row>
     <row r="3" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
-        <v>316</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37" t="s">
+      <c r="B4" s="43" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39" t="s">
-        <v>317</v>
-      </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="O4" s="47" t="s">
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="O4" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="47"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
     </row>
     <row r="5" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
@@ -16239,22 +16273,22 @@
         <f t="shared" si="0"/>
         <v>E0</v>
       </c>
-      <c r="O5" s="46" t="s">
+      <c r="O5" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="35" t="str">
+      <c r="P5" s="35"/>
+      <c r="Q5" s="34" t="str">
         <f>CONCATENATE(B5,B6,B7,B8,C5,C6,C7,C8,D5,D6,D7,D8,E5,E6,E7,E8)</f>
         <v>3925841D02DC09FBDC118597196A0B32</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
     </row>
     <row r="6" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
@@ -16297,22 +16331,22 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35" t="str">
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34" t="str">
         <f>CONCATENATE(F5,F6,F7,F8,G5,G6,G7,G8,H5,H6,H7,H8,I5,I6,I7,I8)</f>
         <v>2B7E151628AED2A6ABF7158809CF4F3C</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
     </row>
     <row r="7" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
@@ -16355,22 +16389,22 @@
         <f t="shared" si="0"/>
         <v>07</v>
       </c>
-      <c r="O7" s="35" t="s">
+      <c r="O7" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35" t="str">
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34" t="str">
         <f>CONCATENATE(J5,J6,J7,J8,K5,K6,K7,K8,L5,L6,L7,L8,M5,M6,M7,M8)</f>
         <v>3243F6A8885A308D313198A2E0370734</v>
       </c>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
     </row>
     <row r="8" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
@@ -16423,42 +16457,42 @@
     </row>
     <row r="10" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="36" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="36" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37" t="s">
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="41" t="s">
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
     </row>
     <row r="11" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -20138,34 +20172,21 @@
       <c r="O55" s="30"/>
       <c r="P55" s="30"/>
       <c r="Q55" s="30"/>
-      <c r="R55" s="42" t="s">
+      <c r="R55" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="S55" s="43"/>
-      <c r="T55" s="43"/>
-      <c r="U55" s="44"/>
-      <c r="V55" s="45" t="s">
+      <c r="S55" s="39"/>
+      <c r="T55" s="39"/>
+      <c r="U55" s="40"/>
+      <c r="V55" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="W55" s="45"/>
-      <c r="X55" s="45"/>
-      <c r="Y55" s="45"/>
+      <c r="W55" s="41"/>
+      <c r="X55" s="41"/>
+      <c r="Y55" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:Y2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="O4:Y4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:Y5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:Y6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:Y7"/>
     <mergeCell ref="R55:U55"/>
     <mergeCell ref="V55:Y55"/>
     <mergeCell ref="B10:E10"/>
@@ -20174,6 +20195,19 @@
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="R10:U10"/>
     <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:Y5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:Y6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:Y7"/>
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:Y2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="O4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20181,7 +20215,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J257"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20208,25 +20242,25 @@
         <v>63</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>64</v>
       </c>
       <c r="F1" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1" s="32" t="s">
         <v>309</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>312</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>